<commit_message>
range update_results added, small fixes
</commit_message>
<xml_diff>
--- a/heta/table1.xlsx
+++ b/heta/table1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12483" uniqueCount="4152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12483" uniqueCount="4153">
   <si>
     <t>on</t>
   </si>
@@ -12473,6 +12473,9 @@
   </si>
   <si>
     <t>delay in math</t>
+  </si>
+  <si>
+    <t>spaceFilter</t>
   </si>
 </sst>
 </file>
@@ -12874,8 +12877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I829"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A590" workbookViewId="0">
+      <selection activeCell="C600" sqref="C600"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21996,8 +21999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J829"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A814" workbookViewId="0">
+      <selection activeCell="D824" sqref="D824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31954,20 +31957,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="580" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A580" s="7">
-        <v>1</v>
-      </c>
-      <c r="B580" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C580" s="7" t="s">
+    <row r="580" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A580" s="8">
+        <v>0</v>
+      </c>
+      <c r="B580" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C580" s="8" t="s">
         <v>598</v>
       </c>
-      <c r="D580" s="7" t="s">
+      <c r="D580" s="8" t="s">
         <v>3898</v>
       </c>
-      <c r="E580" s="7" t="s">
+      <c r="E580" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -33852,23 +33855,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="689" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A689" s="8">
-        <v>1</v>
-      </c>
-      <c r="B689" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C689" s="8" t="s">
+    <row r="689" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A689" s="7">
+        <v>1</v>
+      </c>
+      <c r="B689" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C689" s="7" t="s">
         <v>707</v>
       </c>
-      <c r="D689" s="8" t="s">
+      <c r="D689" s="7" t="s">
         <v>4007</v>
       </c>
-      <c r="E689" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F689" s="8" t="s">
+      <c r="E689" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F689" s="7" t="s">
         <v>4148</v>
       </c>
     </row>
@@ -36304,7 +36307,7 @@
   <dimension ref="A1:J829"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36324,7 +36327,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>4152</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -56167,7 +56170,7 @@
   <dimension ref="A1:E829"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56184,7 +56187,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>4152</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>

</xml_diff>